<commit_message>
changed inputs acc to Judith's comments
</commit_message>
<xml_diff>
--- a/Resources/18_19/Input1_Refactored.xlsx
+++ b/Resources/18_19/Input1_Refactored.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="1160" yWindow="2180" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="107">
   <si>
     <t>Course Name</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>Facing History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS PE </t>
   </si>
 </sst>
 </file>
@@ -352,6 +355,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,8 +398,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -437,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -456,6 +468,10 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -474,6 +490,10 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -803,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1076,6 +1096,9 @@
       <c r="E15">
         <v>22</v>
       </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
       <c r="G15" t="s">
         <v>67</v>
       </c>
@@ -1101,6 +1124,12 @@
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>22</v>
+      </c>
       <c r="G17" t="s">
         <v>74</v>
       </c>
@@ -1137,8 +1166,11 @@
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F20" t="s">
-        <v>56</v>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>22</v>
       </c>
       <c r="G20" t="s">
         <v>67</v>
@@ -1204,6 +1236,15 @@
       <c r="A25" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
@@ -1226,6 +1267,12 @@
       <c r="A27" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>22</v>
+      </c>
       <c r="F27" t="s">
         <v>57</v>
       </c>
@@ -1241,7 +1288,7 @@
         <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1290,6 +1337,12 @@
       <c r="A32" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>22</v>
+      </c>
       <c r="G32" t="s">
         <v>71</v>
       </c>
@@ -1298,6 +1351,12 @@
       <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>22</v>
+      </c>
       <c r="G33" t="s">
         <v>74</v>
       </c>
@@ -1465,9 +1524,6 @@
       <c r="E43">
         <v>22</v>
       </c>
-      <c r="F43" t="s">
-        <v>54</v>
-      </c>
       <c r="G43" t="s">
         <v>70</v>
       </c>
@@ -1479,6 +1535,12 @@
       <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>22</v>
+      </c>
       <c r="G44" t="s">
         <v>74</v>
       </c>
@@ -1490,6 +1552,12 @@
       <c r="C45" t="s">
         <v>78</v>
       </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45">
+        <v>22</v>
+      </c>
       <c r="F45" t="s">
         <v>59</v>
       </c>
@@ -1515,6 +1583,15 @@
       <c r="B47">
         <v>2</v>
       </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>22</v>
+      </c>
+      <c r="F47" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
@@ -1580,6 +1657,12 @@
       <c r="A51" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="D51">
+        <v>10</v>
+      </c>
+      <c r="E51">
+        <v>22</v>
+      </c>
       <c r="F51" t="s">
         <v>61</v>
       </c>
@@ -1588,6 +1671,12 @@
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>22</v>
+      </c>
       <c r="F52" t="s">
         <v>57</v>
       </c>
@@ -1596,6 +1685,12 @@
       <c r="A53" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>22</v>
+      </c>
       <c r="G53" t="s">
         <v>70</v>
       </c>
@@ -1740,6 +1835,12 @@
       <c r="A62" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="D62">
+        <v>10</v>
+      </c>
+      <c r="E62">
+        <v>22</v>
+      </c>
       <c r="F62" t="s">
         <v>58</v>
       </c>
@@ -1748,6 +1849,12 @@
       <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>22</v>
+      </c>
       <c r="F63" t="s">
         <v>61</v>
       </c>
@@ -1790,6 +1897,12 @@
       <c r="A66" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="D66">
+        <v>10</v>
+      </c>
+      <c r="E66">
+        <v>22</v>
+      </c>
       <c r="F66" t="s">
         <v>58</v>
       </c>
@@ -1818,6 +1931,12 @@
       <c r="A68" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
+      <c r="E68">
+        <v>22</v>
+      </c>
       <c r="G68" t="s">
         <v>71</v>
       </c>
@@ -1843,6 +1962,12 @@
       <c r="A70" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="D70">
+        <v>10</v>
+      </c>
+      <c r="E70">
+        <v>22</v>
+      </c>
       <c r="G70" t="s">
         <v>74</v>
       </c>
@@ -1859,6 +1984,23 @@
       </c>
       <c r="G71" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>22</v>
+      </c>
+      <c r="F72" t="s">
+        <v>55</v>
+      </c>
+      <c r="I72" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed empty and other
</commit_message>
<xml_diff>
--- a/Resources/18_19/Input1_Refactored.xlsx
+++ b/Resources/18_19/Input1_Refactored.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$I$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$I$89</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="106">
   <si>
     <t>Course Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>MS/HS PE</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>6th Grade Art</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Drawing and Painting</t>
   </si>
   <si>
-    <t>Empty</t>
-  </si>
-  <si>
     <t>English Seminar</t>
   </si>
   <si>
@@ -205,9 +199,6 @@
   </si>
   <si>
     <t>J</t>
-  </si>
-  <si>
-    <t>Z</t>
   </si>
   <si>
     <t>HS Category</t>
@@ -838,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -859,30 +850,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -891,15 +882,15 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -908,15 +899,15 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -925,18 +916,18 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4">
         <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -945,18 +936,18 @@
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -968,12 +959,12 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -982,12 +973,12 @@
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -996,15 +987,15 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -1013,7 +1004,7 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H9">
         <v>9</v>
@@ -1033,7 +1024,7 @@
         <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1050,15 +1041,15 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1067,12 +1058,12 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1081,15 +1072,15 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1098,12 +1089,12 @@
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1115,15 +1106,15 @@
         <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -1132,15 +1123,15 @@
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -1149,12 +1140,12 @@
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -1163,12 +1154,12 @@
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -1177,12 +1168,12 @@
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -1191,12 +1182,12 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>10</v>
@@ -1205,15 +1196,15 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -1222,23 +1213,26 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23">
         <v>10</v>
       </c>
       <c r="E23">
         <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -1247,12 +1241,15 @@
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="I24" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -1260,16 +1257,19 @@
       <c r="E25">
         <v>22</v>
       </c>
-      <c r="G25" t="s">
-        <v>67</v>
+      <c r="F25" t="s">
+        <v>49</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -1277,19 +1277,13 @@
       <c r="E26">
         <v>22</v>
       </c>
-      <c r="F26" t="s">
-        <v>51</v>
-      </c>
-      <c r="I26" t="s">
-        <v>78</v>
+      <c r="G26" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -1297,13 +1291,13 @@
       <c r="E27">
         <v>22</v>
       </c>
-      <c r="G27" t="s">
-        <v>66</v>
+      <c r="F27" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -1312,12 +1306,15 @@
         <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="I28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29">
         <v>10</v>
@@ -1326,15 +1323,12 @@
         <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30">
         <v>10</v>
@@ -1343,12 +1337,12 @@
         <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31">
         <v>10</v>
@@ -1356,13 +1350,16 @@
       <c r="E31">
         <v>22</v>
       </c>
-      <c r="F31" t="s">
-        <v>57</v>
+      <c r="G31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="D32">
         <v>10</v>
@@ -1371,15 +1368,12 @@
         <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>67</v>
-      </c>
-      <c r="I32" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D33">
         <v>10</v>
@@ -1393,7 +1387,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>10</v>
@@ -1402,12 +1396,15 @@
         <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -1416,15 +1413,15 @@
         <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="I35" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D36">
         <v>10</v>
@@ -1433,15 +1430,12 @@
         <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>63</v>
-      </c>
-      <c r="I36" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="D37">
         <v>10</v>
@@ -1450,12 +1444,12 @@
         <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="D38">
         <v>10</v>
@@ -1464,12 +1458,18 @@
         <v>22</v>
       </c>
       <c r="G38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
       </c>
       <c r="D39">
         <v>10</v>
@@ -1477,39 +1477,33 @@
       <c r="E39">
         <v>22</v>
       </c>
-      <c r="G39" t="s">
-        <v>65</v>
+      <c r="F39" t="s">
+        <v>57</v>
+      </c>
+      <c r="H39">
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
-      <c r="C40" t="s">
-        <v>75</v>
-      </c>
       <c r="D40">
         <v>10</v>
       </c>
       <c r="E40">
         <v>22</v>
       </c>
-      <c r="F40" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40">
-        <v>6</v>
+      <c r="G40" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D41">
         <v>10</v>
@@ -1517,13 +1511,19 @@
       <c r="E41">
         <v>22</v>
       </c>
+      <c r="F41" t="s">
+        <v>55</v>
+      </c>
       <c r="G41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
       </c>
       <c r="D42">
         <v>10</v>
@@ -1532,18 +1532,15 @@
         <v>22</v>
       </c>
       <c r="F42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D43">
         <v>10</v>
@@ -1551,16 +1548,16 @@
       <c r="E43">
         <v>22</v>
       </c>
-      <c r="F43" t="s">
-        <v>57</v>
-      </c>
       <c r="G43" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="I43" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="D44">
         <v>10</v>
@@ -1569,15 +1566,15 @@
         <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>67</v>
-      </c>
-      <c r="I44" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -1585,16 +1582,13 @@
       <c r="E45">
         <v>22</v>
       </c>
-      <c r="G45" t="s">
-        <v>71</v>
+      <c r="F45" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="D46">
         <v>10</v>
@@ -1603,12 +1597,12 @@
         <v>22</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="D47">
         <v>10</v>
@@ -1617,12 +1611,15 @@
         <v>22</v>
       </c>
       <c r="F47" t="s">
-        <v>60</v>
+        <v>50</v>
+      </c>
+      <c r="I47" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48">
         <v>10</v>
@@ -1631,15 +1628,15 @@
         <v>22</v>
       </c>
       <c r="F48" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I48" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -1648,15 +1645,18 @@
         <v>22</v>
       </c>
       <c r="F49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>103</v>
+        <v>7</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
       </c>
       <c r="D50">
         <v>10</v>
@@ -1665,18 +1665,18 @@
         <v>22</v>
       </c>
       <c r="F50" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="G50" t="s">
+        <v>60</v>
       </c>
       <c r="I50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D51">
         <v>10</v>
@@ -1685,18 +1685,18 @@
         <v>22</v>
       </c>
       <c r="F51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G51" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D52">
         <v>10</v>
@@ -1705,18 +1705,15 @@
         <v>22</v>
       </c>
       <c r="F52" t="s">
-        <v>55</v>
-      </c>
-      <c r="G52" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="D53">
         <v>10</v>
@@ -1725,15 +1722,12 @@
         <v>22</v>
       </c>
       <c r="F53" t="s">
-        <v>55</v>
-      </c>
-      <c r="I53" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -1742,12 +1736,12 @@
         <v>22</v>
       </c>
       <c r="F54" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D55">
         <v>10</v>
@@ -1755,13 +1749,22 @@
       <c r="E55">
         <v>22</v>
       </c>
-      <c r="F55" t="s">
-        <v>54</v>
+      <c r="G55" t="s">
+        <v>64</v>
+      </c>
+      <c r="I55" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>95</v>
+        <v>38</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
       </c>
       <c r="D56">
         <v>10</v>
@@ -1769,19 +1772,16 @@
       <c r="E56">
         <v>22</v>
       </c>
-      <c r="G56" t="s">
-        <v>67</v>
-      </c>
-      <c r="I56" t="s">
-        <v>78</v>
+      <c r="F56" t="s">
+        <v>54</v>
+      </c>
+      <c r="H56">
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D57">
         <v>10</v>
@@ -1789,34 +1789,28 @@
       <c r="E57">
         <v>22</v>
       </c>
-      <c r="F57" t="s">
-        <v>61</v>
-      </c>
       <c r="G57" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="I57" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B58">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s">
-        <v>75</v>
-      </c>
       <c r="D58">
         <v>10</v>
       </c>
       <c r="E58">
         <v>22</v>
       </c>
-      <c r="F58" t="s">
-        <v>56</v>
-      </c>
-      <c r="H58">
-        <v>6</v>
+      <c r="G58" t="s">
+        <v>66</v>
+      </c>
+      <c r="I58" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1830,10 +1824,10 @@
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -1847,10 +1841,7 @@
         <v>22</v>
       </c>
       <c r="G60" t="s">
-        <v>69</v>
-      </c>
-      <c r="I60" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1864,15 +1855,12 @@
         <v>22</v>
       </c>
       <c r="G61" t="s">
-        <v>69</v>
-      </c>
-      <c r="I61" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="D62">
         <v>10</v>
@@ -1880,13 +1868,13 @@
       <c r="E62">
         <v>22</v>
       </c>
-      <c r="G62" t="s">
-        <v>64</v>
+      <c r="F62" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="D63">
         <v>10</v>
@@ -1894,13 +1882,16 @@
       <c r="E63">
         <v>22</v>
       </c>
-      <c r="G63" t="s">
-        <v>64</v>
+      <c r="F63" t="s">
+        <v>53</v>
+      </c>
+      <c r="I63" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D64">
         <v>10</v>
@@ -1909,12 +1900,15 @@
         <v>22</v>
       </c>
       <c r="F64" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>92</v>
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
       </c>
       <c r="D65">
         <v>10</v>
@@ -1925,13 +1919,13 @@
       <c r="F65" t="s">
         <v>55</v>
       </c>
-      <c r="I65" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>106</v>
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
       </c>
       <c r="D66">
         <v>10</v>
@@ -1940,15 +1934,12 @@
         <v>22</v>
       </c>
       <c r="F66" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="D67">
         <v>10</v>
@@ -1957,15 +1948,18 @@
         <v>22</v>
       </c>
       <c r="F67" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="G67" t="s">
+        <v>66</v>
+      </c>
+      <c r="I67" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="D68">
         <v>10</v>
@@ -1973,13 +1967,16 @@
       <c r="E68">
         <v>22</v>
       </c>
-      <c r="F68" t="s">
-        <v>57</v>
+      <c r="G68" t="s">
+        <v>66</v>
+      </c>
+      <c r="I68" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D69">
         <v>10</v>
@@ -1987,19 +1984,13 @@
       <c r="E69">
         <v>22</v>
       </c>
-      <c r="F69" t="s">
-        <v>55</v>
-      </c>
       <c r="G69" t="s">
-        <v>69</v>
-      </c>
-      <c r="I69" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D70">
         <v>10</v>
@@ -2008,15 +1999,12 @@
         <v>22</v>
       </c>
       <c r="G70" t="s">
-        <v>69</v>
-      </c>
-      <c r="I70" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D71">
         <v>10</v>
@@ -2030,7 +2018,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D72">
         <v>10</v>
@@ -2039,39 +2027,11 @@
         <v>22</v>
       </c>
       <c r="G72" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D73">
-        <v>10</v>
-      </c>
-      <c r="E73">
-        <v>22</v>
-      </c>
-      <c r="G73" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D74">
-        <v>10</v>
-      </c>
-      <c r="E74">
-        <v>22</v>
-      </c>
-      <c r="G74" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I91">
+  <autoFilter ref="A1:I89">
     <sortState ref="A2:I73">
       <sortCondition ref="A1:A90"/>
     </sortState>

</xml_diff>